<commit_message>
Added a new sheet for exam 25 June
</commit_message>
<xml_diff>
--- a/Session13_Ta/Practical13.xlsx
+++ b/Session13_Ta/Practical13.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sina\Documents\GitHub\CCRE_Fall_2023\Session13_Ta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DFCF55-F09D-4AF2-9720-391D216AB151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722DA3CB-B1A9-42A2-906E-09FB802EAC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" activeTab="1" xr2:uid="{D8C94763-68ED-4754-B889-67D69145CD04}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ex2 (2)" sheetId="9" r:id="rId2"/>
     <sheet name="ex2" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1.0000000000000001E-9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="43">
   <si>
     <t>K</t>
   </si>
@@ -151,9 +151,6 @@
     <t>length</t>
   </si>
   <si>
-    <t>2nd condition</t>
-  </si>
-  <si>
     <t>3rd condition</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>r/CA2</t>
+  </si>
+  <si>
+    <t>CB</t>
   </si>
 </sst>
 </file>
@@ -1177,19 +1177,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.32553264167086327</c:v>
+                  <c:v>1.2840454199239584</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32553264167086232</c:v>
+                  <c:v>1.2659602731644684</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3255326416708641</c:v>
+                  <c:v>1.247875126404975</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32553264167086376</c:v>
+                  <c:v>1.2478751264049728</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32553264167086282</c:v>
+                  <c:v>1.229789979645483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1233,48 +1233,48 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ex2 (2)'!$F$17:$F$21</c:f>
+              <c:f>'ex2 (2)'!$F$24:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ex2 (2)'!$M$17:$M$21</c:f>
+              <c:f>'ex2 (2)'!$M$24:$M$28</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.60223538709109714</c:v>
+                  <c:v>0.73847682601260534</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59680984306324836</c:v>
+                  <c:v>0.63298013658223362</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58130828869797024</c:v>
+                  <c:v>0.55046665449204935</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57985501797622563</c:v>
+                  <c:v>0.48628950175524016</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57872469630375734</c:v>
+                  <c:v>0.66249409136334969</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1318,7 +1318,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ex2 (2)'!$F$27:$F$31</c:f>
+              <c:f>'ex2 (2)'!$F$40:$F$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1342,24 +1342,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ex2 (2)'!$M$27:$M$31</c:f>
+              <c:f>'ex2 (2)'!$M$40:$M$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.81383160417715827</c:v>
+                  <c:v>0.90425733797462016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81383160417715839</c:v>
+                  <c:v>0.90425733797462027</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.80220543840319836</c:v>
+                  <c:v>0.89133937600355362</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79348581407272856</c:v>
+                  <c:v>0.88165090452525385</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78670388403791813</c:v>
+                  <c:v>0.87411542670879772</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1913,7 +1913,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-1.1222925407304634</c:v>
+                  <c:v>0.19202832076433624</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-0.52763274208237199</c:v>
@@ -6426,16 +6426,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>486573</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>11906</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>451620</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>3167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>546105</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>121443</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>511151</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>112705</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6547,9 +6547,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6587,7 +6587,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6693,7 +6693,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6835,7 +6835,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8058,7 +8058,7 @@
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8078,13 +8078,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4">
         <v>1750</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -8169,6 +8169,9 @@
         <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -8181,30 +8184,34 @@
       </c>
       <c r="G8" s="2">
         <f xml:space="preserve"> (1-L8/100)*F8</f>
-        <v>0.98</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="H8">
         <f xml:space="preserve"> G8-F8</f>
-        <v>-2.0000000000000018E-2</v>
+        <v>-7.0999999999999952E-2</v>
       </c>
       <c r="I8" s="4">
         <f xml:space="preserve"> H8/$B$11</f>
-        <v>-341.80927375440643</v>
+        <v>-1348.2476909201564</v>
       </c>
       <c r="J8" s="6">
         <f xml:space="preserve"> -I8/((1-$B$4)*$B$2)</f>
-        <v>0.32553264167086327</v>
+        <v>1.2840454199239584</v>
       </c>
       <c r="K8" s="6">
         <f xml:space="preserve"> J8/F8</f>
-        <v>0.32553264167086327</v>
+        <v>1.2840454199239584</v>
       </c>
       <c r="L8" s="7">
-        <v>2</v>
+        <v>7.1</v>
       </c>
       <c r="M8">
-        <f xml:space="preserve"> J8/F8^2</f>
-        <v>0.32553264167086327</v>
+        <f xml:space="preserve"> J8/F8</f>
+        <v>1.2840454199239584</v>
+      </c>
+      <c r="N8" s="6">
+        <f xml:space="preserve"> $B$11*J8 + 0</f>
+        <v>6.7619047619047558E-5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -8212,7 +8219,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -8224,31 +8231,35 @@
         <v>1.2</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" ref="G9:G12" si="0" xml:space="preserve"> (1-L9/100)*F9</f>
-        <v>1.1712</v>
+        <f t="shared" ref="G9:G17" si="0" xml:space="preserve"> (1-L9/100)*F9</f>
+        <v>1.1159999999999999</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:H12" si="1" xml:space="preserve"> G9-F9</f>
-        <v>-2.8799999999999937E-2</v>
+        <f t="shared" ref="H9:H17" si="1" xml:space="preserve"> G9-F9</f>
+        <v>-8.4000000000000075E-2</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" ref="I9:I12" si="2" xml:space="preserve"> H9/$B$11</f>
-        <v>-492.20535420634377</v>
+        <f t="shared" ref="I9:I17" si="2" xml:space="preserve"> H9/$B$11</f>
+        <v>-1595.10994418723</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" ref="J9:J12" si="3" xml:space="preserve"> -I9/((1-$B$4)*$B$2)</f>
-        <v>0.46876700400604171</v>
+        <f t="shared" ref="J9:J17" si="3" xml:space="preserve"> -I9/((1-$B$4)*$B$2)</f>
+        <v>1.519152327797362</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" ref="K9:K12" si="4" xml:space="preserve"> J9/F9</f>
-        <v>0.39063917000503479</v>
+        <f t="shared" ref="K9:K17" si="4" xml:space="preserve"> J9/F9</f>
+        <v>1.2659602731644684</v>
       </c>
       <c r="L9" s="7">
-        <v>2.4</v>
+        <v>7</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:M12" si="5" xml:space="preserve"> J9/F9^2</f>
-        <v>0.32553264167086232</v>
+        <f t="shared" ref="M9:M17" si="5" xml:space="preserve"> J9/F9</f>
+        <v>1.2659602731644684</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" ref="N9:N17" si="6" xml:space="preserve"> $B$11*J9 + 0</f>
+        <v>8.0000000000000074E-5</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -8257,7 +8268,7 @@
       </c>
       <c r="B10" s="4">
         <f>B7*B9/298</f>
-        <v>0.12080536912751678</v>
+        <v>0.13422818791946309</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -8270,30 +8281,34 @@
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>1.3607999999999998</v>
+        <v>1.3033999999999999</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>-3.9200000000000124E-2</v>
+        <v>-9.6600000000000019E-2</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="2"/>
-        <v>-669.94617655863817</v>
+        <v>-1834.3764358153132</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="3"/>
-        <v>0.63804397767489351</v>
+        <v>1.7470251769669649</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="4"/>
-        <v>0.45574569833920969</v>
+        <v>1.247875126404975</v>
       </c>
       <c r="L10" s="7">
-        <v>2.8</v>
+        <v>6.9</v>
       </c>
       <c r="M10">
         <f t="shared" si="5"/>
-        <v>0.3255326416708641</v>
+        <v>1.247875126404975</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" si="6"/>
+        <v>9.2000000000000014E-5</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -8302,7 +8317,7 @@
       </c>
       <c r="B11" s="4">
         <f>$B$3/B10</f>
-        <v>5.8512163173109889E-5</v>
+        <v>5.2660946855798907E-5</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -8315,30 +8330,34 @@
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>1.5488</v>
+        <v>1.4896000000000003</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>-5.1200000000000134E-2</v>
+        <v>-0.11039999999999983</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="2"/>
-        <v>-875.03174081128202</v>
+        <v>-2096.4302123603543</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="3"/>
-        <v>0.83336356267741141</v>
+        <v>1.9966002022479565</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" si="4"/>
-        <v>0.52085222667338205</v>
+        <v>1.2478751264049728</v>
       </c>
       <c r="L11" s="7">
-        <v>3.2</v>
+        <v>6.9</v>
       </c>
       <c r="M11">
         <f t="shared" si="5"/>
-        <v>0.32553264167086376</v>
+        <v>1.2478751264049728</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="6"/>
+        <v>1.0514285714285699E-4</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -8350,690 +8369,966 @@
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>1.7352000000000001</v>
+        <v>1.6776</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>-6.4799999999999969E-2</v>
+        <v>-0.12240000000000006</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="2"/>
-        <v>-1107.4620469642755</v>
+        <v>-2324.3030615299626</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="3"/>
-        <v>1.0547257590135957</v>
+        <v>2.2136219633618692</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" si="4"/>
-        <v>0.58595875500755312</v>
+        <v>1.229789979645483</v>
       </c>
       <c r="L12" s="7">
-        <v>3.6</v>
+        <v>6.8</v>
       </c>
       <c r="M12">
         <f t="shared" si="5"/>
-        <v>0.32553264167086282</v>
+        <v>1.229789979645483</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="6"/>
+        <v>1.1657142857142864E-4</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E13" s="2">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8660000000000001</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>-0.1339999999999999</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="2"/>
+        <v>-2544.5801490605768</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="3"/>
+        <v>2.4234096657719779</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="4"/>
+        <v>1.211704832885989</v>
+      </c>
+      <c r="L13" s="7">
+        <v>6.7</v>
+      </c>
       <c r="M13">
-        <f xml:space="preserve"> AVERAGE(M8:M12)</f>
-        <v>0.32553264167086327</v>
+        <f t="shared" si="5"/>
+        <v>1.211704832885989</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2761904761904753E-4</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
+      <c r="E14" s="2">
+        <v>7</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0526000000000004</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>-0.14739999999999975</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="2"/>
+        <v>-2799.0381639666321</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="3"/>
+        <v>2.6657506323491735</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2117048328859878</v>
+      </c>
+      <c r="L14" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="5"/>
+        <v>1.2117048328859878</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="6"/>
+        <v>1.4038095238095216E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E15" s="2">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2415999999999996</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>-0.15840000000000032</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="2"/>
+        <v>-3007.9216090387799</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="3"/>
+        <v>2.8646872467035998</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1936196861265</v>
+      </c>
+      <c r="L15" s="7">
+        <v>6.6</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="5"/>
+        <v>1.1936196861265</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="6"/>
+        <v>1.5085714285714317E-4</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16">
-        <v>0.1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" s="1"/>
+      <c r="E16" s="2">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>2.431</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>-0.16900000000000004</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="2"/>
+        <v>-3209.2092924719245</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="3"/>
+        <v>3.056389802354214</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1755345393670054</v>
+      </c>
+      <c r="L16" s="7">
+        <v>6.5</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="5"/>
+        <v>1.1755345393670054</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="6"/>
+        <v>1.6095238095238098E-4</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E17" s="2">
+        <v>10</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6179999999999999</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>-0.18199999999999994</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="2"/>
+        <v>-3456.0715457389938</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="3"/>
+        <v>3.2914967102276131</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1755345393670047</v>
+      </c>
+      <c r="L17" s="7">
+        <v>6.5</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="5"/>
+        <v>1.1755345393670047</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="6"/>
+        <v>1.7333333333333328E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f xml:space="preserve"> AVERAGE(M8:M17)</f>
+        <v>1.2243644356176344</v>
+      </c>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <f xml:space="preserve"> 0.08</f>
+        <v>0.08</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="2">
+      <c r="M22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E23" s="2">
         <v>1</v>
       </c>
-      <c r="G17" s="2">
-        <f xml:space="preserve"> (1-L17/100)*F17</f>
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="H17">
-        <f xml:space="preserve"> G17-F17</f>
-        <v>-3.7000000000000033E-2</v>
-      </c>
-      <c r="I17" s="4">
-        <f xml:space="preserve"> H17/$B$11</f>
-        <v>-632.34715644565199</v>
-      </c>
-      <c r="J17" s="6">
-        <f xml:space="preserve"> -I17/((1-$B$4)*$B$2)</f>
-        <v>0.60223538709109714</v>
-      </c>
-      <c r="K17" s="6">
-        <f xml:space="preserve"> J17/F17</f>
-        <v>0.60223538709109714</v>
-      </c>
-      <c r="L17" s="7">
-        <v>3.7</v>
-      </c>
-      <c r="M17" s="6">
-        <f xml:space="preserve"> J17/F17^2</f>
-        <v>0.60223538709109714</v>
-      </c>
-      <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>480</v>
-      </c>
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" ref="G18:G21" si="6" xml:space="preserve"> (1-L18/100)*F18</f>
-        <v>1.1472</v>
-      </c>
-      <c r="H18">
-        <f t="shared" ref="H18:H21" si="7" xml:space="preserve"> G18-F18</f>
-        <v>-5.2799999999999958E-2</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" ref="I18:I21" si="8" xml:space="preserve"> H18/$B$11</f>
-        <v>-902.37648271163152</v>
-      </c>
-      <c r="J18" s="6">
-        <f t="shared" ref="J18:J21" si="9" xml:space="preserve"> -I18/((1-$B$4)*$B$2)</f>
-        <v>0.85940617401107766</v>
-      </c>
-      <c r="K18" s="6">
-        <f t="shared" ref="K18:K21" si="10" xml:space="preserve"> J18/F18</f>
-        <v>0.71617181167589805</v>
-      </c>
-      <c r="L18" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M18" s="6">
-        <f t="shared" ref="M18:M21" si="11" xml:space="preserve"> J18/F18^2</f>
-        <v>0.59680984306324836</v>
-      </c>
-      <c r="N18" s="7"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4">
-        <f>B16*B18/298</f>
-        <v>0.16107382550335569</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="2">
-        <v>3</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="6"/>
-        <v>1.3299999999999998</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="7"/>
-        <v>-7.0000000000000062E-2</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="8"/>
-        <v>-1196.3324581404227</v>
-      </c>
-      <c r="J19" s="6">
-        <f t="shared" si="9"/>
-        <v>1.1393642458480215</v>
-      </c>
-      <c r="K19" s="6">
-        <f t="shared" si="10"/>
-        <v>0.81383160417715827</v>
-      </c>
-      <c r="L19" s="7">
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <f xml:space="preserve"> (1-L23/100)*F23</f>
+        <v>0.95</v>
+      </c>
+      <c r="H23">
+        <f xml:space="preserve"> G23-F23</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="I23" s="4">
+        <f xml:space="preserve"> H23/$B$11</f>
+        <v>-949.47020487335112</v>
+      </c>
+      <c r="J23" s="6">
+        <f xml:space="preserve"> -I23/((1-$B$4)*$B$2)</f>
+        <v>0.90425733797462016</v>
+      </c>
+      <c r="K23" s="6">
+        <f xml:space="preserve"> J23/F23</f>
+        <v>0.90425733797462016</v>
+      </c>
+      <c r="L23" s="7">
         <v>5</v>
       </c>
-      <c r="M19" s="6">
-        <f t="shared" si="11"/>
-        <v>0.58130828869797024</v>
-      </c>
-      <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4">
-        <f>$B$3/B19</f>
-        <v>4.3884122379832426E-5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="2">
-        <v>4</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="6"/>
-        <v>1.5087999999999999</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="7"/>
-        <v>-9.120000000000017E-2</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="8"/>
-        <v>-1558.6502883200949</v>
-      </c>
-      <c r="J20" s="6">
-        <f t="shared" si="9"/>
-        <v>1.4844288460191379</v>
-      </c>
-      <c r="K20" s="6">
-        <f t="shared" si="10"/>
-        <v>0.92776802876196118</v>
-      </c>
-      <c r="L20" s="7">
-        <v>5.7</v>
-      </c>
-      <c r="M20" s="6">
-        <f t="shared" si="11"/>
-        <v>0.57985501797622563</v>
-      </c>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E21" s="2">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="6"/>
-        <v>1.6847999999999999</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="7"/>
-        <v>-0.11520000000000019</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="8"/>
-        <v>-1968.8214168253826</v>
-      </c>
-      <c r="J21" s="6">
-        <f t="shared" si="9"/>
-        <v>1.8750680160241739</v>
-      </c>
-      <c r="K21" s="6">
-        <f t="shared" si="10"/>
-        <v>1.0417044533467632</v>
-      </c>
-      <c r="L21" s="7">
-        <v>6.4</v>
-      </c>
-      <c r="M21" s="6">
-        <f t="shared" si="11"/>
-        <v>0.57872469630375734</v>
-      </c>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L22" s="6"/>
-      <c r="M22" s="6">
-        <f xml:space="preserve"> AVERAGE(M17:M21)</f>
-        <v>0.58778664662645974</v>
-      </c>
-      <c r="N22" s="4"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="M23">
+        <f xml:space="preserve"> J23/F23^2</f>
+        <v>0.90425733797462016</v>
+      </c>
+      <c r="N23" s="6">
+        <f>J23*$B$26+0.25</f>
+        <v>0.25004761904761907</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="M24" s="8"/>
-      <c r="N24" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>500</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" ref="G24:G32" si="7" xml:space="preserve"> (1-L24/100)*F24</f>
+        <v>1.1412</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24:H32" si="8" xml:space="preserve"> G24-F24</f>
+        <v>-5.8799999999999963E-2</v>
+      </c>
+      <c r="I24" s="4">
+        <f t="shared" ref="I24:I32" si="9" xml:space="preserve"> H24/$B$11</f>
+        <v>-1116.5769609310591</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" ref="J24:J32" si="10" xml:space="preserve"> -I24/((1-$B$4)*$B$2)</f>
+        <v>1.0634066294581517</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" ref="K24:K32" si="11" xml:space="preserve"> J24/F24</f>
+        <v>0.88617219121512647</v>
+      </c>
+      <c r="L24" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M27" si="12" xml:space="preserve"> J24/F24^2</f>
+        <v>0.73847682601260534</v>
+      </c>
+      <c r="N24" s="6">
+        <f t="shared" ref="N24:N32" si="13">J24*$B$26+0.25</f>
+        <v>0.250056</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M25" s="6"/>
-      <c r="N25" s="7"/>
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="4">
+        <f>B22*B24/298</f>
+        <v>0.13422818791946309</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="7"/>
+        <v>1.3313999999999999</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="8"/>
+        <v>-6.8599999999999994E-2</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="9"/>
+        <v>-1302.6731210862365</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="10"/>
+        <v>1.2406410677011777</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="11"/>
+        <v>0.88617219121512691</v>
+      </c>
+      <c r="L25" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="12"/>
+        <v>0.63298013658223362</v>
+      </c>
+      <c r="N25" s="6">
+        <f t="shared" si="13"/>
+        <v>0.25006533333333331</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26">
-        <v>0.15</v>
+        <v>19</v>
+      </c>
+      <c r="B26" s="4">
+        <f>$B$3/B25</f>
+        <v>5.2660946855798907E-5</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N26" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="7"/>
+        <v>1.5220800000000001</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="8"/>
+        <v>-7.7919999999999989E-2</v>
+      </c>
+      <c r="I26" s="4">
+        <f t="shared" si="9"/>
+        <v>-1479.6543672746288</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="10"/>
+        <v>1.4091946354996465</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" si="11"/>
+        <v>0.88074664718727902</v>
+      </c>
+      <c r="L26" s="7">
+        <v>4.87</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="12"/>
+        <v>0.55046665449204935</v>
+      </c>
+      <c r="N26" s="6">
+        <f t="shared" si="13"/>
+        <v>0.25007420952380954</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E27" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F27" s="2">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="G27" s="2">
-        <f xml:space="preserve"> (1-L27/100)*F27</f>
-        <v>0.95</v>
+        <f t="shared" si="7"/>
+        <v>1.71288</v>
       </c>
       <c r="H27">
-        <f xml:space="preserve"> G27-F27</f>
-        <v>-5.0000000000000044E-2</v>
+        <f t="shared" si="8"/>
+        <v>-8.7120000000000086E-2</v>
       </c>
       <c r="I27" s="4">
-        <f xml:space="preserve"> H27/$B$11</f>
-        <v>-854.52318438601617</v>
+        <f t="shared" si="9"/>
+        <v>-1654.3568849713272</v>
       </c>
       <c r="J27" s="6">
-        <f xml:space="preserve"> -I27/((1-$B$4)*$B$2)</f>
-        <v>0.81383160417715827</v>
+        <f t="shared" si="10"/>
+        <v>1.5755779856869783</v>
       </c>
       <c r="K27" s="6">
-        <f xml:space="preserve"> J27/F27</f>
-        <v>0.81383160417715827</v>
+        <f t="shared" si="11"/>
+        <v>0.87532110315943235</v>
       </c>
       <c r="L27" s="7">
-        <v>5</v>
-      </c>
-      <c r="M27" s="6">
-        <f xml:space="preserve"> J27/F27^2</f>
-        <v>0.81383160417715827</v>
-      </c>
-      <c r="N27" s="7"/>
+        <v>4.84</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="12"/>
+        <v>0.48628950175524016</v>
+      </c>
+      <c r="N27" s="6">
+        <f t="shared" si="13"/>
+        <v>0.25008297142857144</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>510</v>
-      </c>
-      <c r="C28" t="s">
-        <v>0</v>
-      </c>
       <c r="E28" s="2">
+        <v>6</v>
+      </c>
+      <c r="F28" s="2">
         <v>2</v>
       </c>
-      <c r="F28" s="2">
-        <v>1.2</v>
-      </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G31" si="12" xml:space="preserve"> (1-L28/100)*F28</f>
-        <v>1.1279999999999999</v>
+        <f t="shared" si="7"/>
+        <v>1.9036</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="H28:H31" si="13" xml:space="preserve"> G28-F28</f>
-        <v>-7.2000000000000064E-2</v>
+        <f t="shared" si="8"/>
+        <v>-9.6400000000000041E-2</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" ref="I28:I31" si="14" xml:space="preserve"> H28/$B$11</f>
-        <v>-1230.5133855158633</v>
+        <f t="shared" si="9"/>
+        <v>-1830.5785549958202</v>
       </c>
       <c r="J28" s="6">
-        <f t="shared" ref="J28:J31" si="15" xml:space="preserve"> -I28/((1-$B$4)*$B$2)</f>
-        <v>1.171917510015108</v>
+        <f t="shared" si="10"/>
+        <v>1.7434081476150669</v>
       </c>
       <c r="K28" s="6">
-        <f t="shared" ref="K28:K31" si="16" xml:space="preserve"> J28/F28</f>
-        <v>0.97659792501259002</v>
+        <f t="shared" si="11"/>
+        <v>0.87170407380753345</v>
       </c>
       <c r="L28" s="7">
-        <v>6</v>
-      </c>
-      <c r="M28" s="6">
-        <f t="shared" ref="M28:M31" si="17" xml:space="preserve"> J28/F28^2</f>
-        <v>0.81383160417715839</v>
-      </c>
-      <c r="N28" s="7"/>
+        <v>4.82</v>
+      </c>
+      <c r="M28">
+        <f xml:space="preserve"> AVERAGE(M23:M27)</f>
+        <v>0.66249409136334969</v>
+      </c>
+      <c r="N28" s="6">
+        <f t="shared" si="13"/>
+        <v>0.25009180952380955</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="4">
-        <f>B26*B28/298</f>
-        <v>0.25671140939597314</v>
-      </c>
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
       <c r="E29" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F29" s="2">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="12"/>
-        <v>1.3033999999999999</v>
+        <f t="shared" si="7"/>
+        <v>2.0946199999999999</v>
       </c>
       <c r="H29">
+        <f t="shared" si="8"/>
+        <v>-0.10538000000000025</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" si="9"/>
+        <v>-2001.1034037910779</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="10"/>
+        <v>1.9058127655153123</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" si="11"/>
+        <v>0.86627852977968733</v>
+      </c>
+      <c r="L29" s="7">
+        <v>4.79</v>
+      </c>
+      <c r="M29">
+        <f xml:space="preserve"> J29/F29^2</f>
+        <v>0.39376296808167605</v>
+      </c>
+      <c r="N29" s="6">
         <f t="shared" si="13"/>
-        <v>-9.6600000000000019E-2</v>
-      </c>
-      <c r="I29" s="4">
-        <f t="shared" si="14"/>
-        <v>-1650.9387922337821</v>
-      </c>
-      <c r="J29" s="6">
-        <f t="shared" si="15"/>
-        <v>1.5723226592702686</v>
-      </c>
-      <c r="K29" s="6">
-        <f t="shared" si="16"/>
-        <v>1.1230876137644776</v>
-      </c>
-      <c r="L29" s="7">
-        <v>6.9</v>
-      </c>
-      <c r="M29" s="6">
-        <f t="shared" si="17"/>
-        <v>0.80220543840319836</v>
-      </c>
-      <c r="N29" s="7"/>
+        <v>0.25010036190476193</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="4">
-        <f>$B$3/B29</f>
-        <v>2.7535135610875244E-5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>21</v>
-      </c>
       <c r="E30" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F30" s="2">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="12"/>
-        <v>1.4752000000000001</v>
+        <f t="shared" si="7"/>
+        <v>2.2857599999999998</v>
       </c>
       <c r="H30">
+        <f t="shared" si="8"/>
+        <v>-0.11424000000000012</v>
+      </c>
+      <c r="I30" s="4">
+        <f t="shared" si="9"/>
+        <v>-2169.3495240946331</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="10"/>
+        <v>2.0660471658044126</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="11"/>
+        <v>0.86085298575183866</v>
+      </c>
+      <c r="L30" s="7">
+        <v>4.76</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ref="M30:M32" si="14" xml:space="preserve"> J30/F30^2</f>
+        <v>0.35868874406326612</v>
+      </c>
+      <c r="N30" s="6">
         <f t="shared" si="13"/>
-        <v>-0.12480000000000002</v>
-      </c>
-      <c r="I30" s="4">
-        <f t="shared" si="14"/>
-        <v>-2132.8898682274948</v>
-      </c>
-      <c r="J30" s="6">
-        <f t="shared" si="15"/>
-        <v>2.0313236840261855</v>
-      </c>
-      <c r="K30" s="6">
-        <f t="shared" si="16"/>
-        <v>1.2695773025163659</v>
-      </c>
-      <c r="L30" s="7">
-        <v>7.8</v>
-      </c>
-      <c r="M30" s="6">
-        <f t="shared" si="17"/>
-        <v>0.79348581407272856</v>
-      </c>
-      <c r="N30" s="4"/>
+        <v>0.25010880000000002</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E31" s="2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F31" s="2">
-        <v>1.8</v>
+        <v>2.6</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="12"/>
-        <v>1.6434000000000002</v>
+        <f t="shared" si="7"/>
+        <v>2.4767600000000001</v>
       </c>
       <c r="H31">
+        <f t="shared" si="8"/>
+        <v>-0.12324000000000002</v>
+      </c>
+      <c r="I31" s="4">
+        <f t="shared" si="9"/>
+        <v>-2340.2541609718342</v>
+      </c>
+      <c r="J31" s="6">
+        <f t="shared" si="10"/>
+        <v>2.2288134866398419</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="11"/>
+        <v>0.85723595639993921</v>
+      </c>
+      <c r="L31" s="7">
+        <v>4.74</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="14"/>
+        <v>0.32970613707689966</v>
+      </c>
+      <c r="N31" s="6">
         <f t="shared" si="13"/>
-        <v>-0.15659999999999985</v>
-      </c>
-      <c r="I31" s="4">
+        <v>0.25011737142857143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+      <c r="F32" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="7"/>
+        <v>2.6681199999999996</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="8"/>
+        <v>-0.13188000000000022</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" si="9"/>
+        <v>-2504.3226123739528</v>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="10"/>
+        <v>2.3850691546418599</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" si="11"/>
+        <v>0.85181041237209287</v>
+      </c>
+      <c r="L32" s="7">
+        <v>4.71</v>
+      </c>
+      <c r="M32">
         <f t="shared" si="14"/>
-        <v>-2676.3666134969976</v>
-      </c>
-      <c r="J31" s="6">
-        <f t="shared" si="15"/>
-        <v>2.5489205842828548</v>
-      </c>
-      <c r="K31" s="6">
-        <f t="shared" si="16"/>
-        <v>1.4160669912682526</v>
-      </c>
-      <c r="L31" s="7">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="M31" s="6">
-        <f t="shared" si="17"/>
-        <v>0.78670388403791813</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="6"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="6"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="6"/>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="6"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="L38" s="6"/>
+        <v>0.30421800441860464</v>
+      </c>
+      <c r="N32" s="6">
+        <f t="shared" si="13"/>
+        <v>0.2501256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="M37" s="8"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M38" s="6"/>
       <c r="N38" s="4"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39">
+        <v>0.15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2">
+        <f xml:space="preserve"> (1-L40/100)*F40</f>
+        <v>0.95</v>
+      </c>
+      <c r="H40">
+        <f xml:space="preserve"> G40-F40</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="I40" s="4">
+        <f xml:space="preserve"> H40/$B$11</f>
+        <v>-949.47020487335112</v>
+      </c>
+      <c r="J40" s="6">
+        <f xml:space="preserve"> -I40/((1-$B$4)*$B$2)</f>
+        <v>0.90425733797462016</v>
+      </c>
+      <c r="K40" s="6">
+        <f xml:space="preserve"> J40/F40</f>
+        <v>0.90425733797462016</v>
+      </c>
+      <c r="L40" s="7">
+        <v>5</v>
+      </c>
+      <c r="M40" s="6">
+        <f xml:space="preserve"> J40/F40^2</f>
+        <v>0.90425733797462016</v>
+      </c>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>510</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" ref="G41:G44" si="15" xml:space="preserve"> (1-L41/100)*F41</f>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ref="H41:H44" si="16" xml:space="preserve"> G41-F41</f>
+        <v>-7.2000000000000064E-2</v>
+      </c>
+      <c r="I41" s="4">
+        <f t="shared" ref="I41:I44" si="17" xml:space="preserve"> H41/$B$11</f>
+        <v>-1367.2370950176257</v>
+      </c>
+      <c r="J41" s="6">
+        <f t="shared" ref="J41:J44" si="18" xml:space="preserve"> -I41/((1-$B$4)*$B$2)</f>
+        <v>1.3021305666834531</v>
+      </c>
+      <c r="K41" s="6">
+        <f t="shared" ref="K41:K44" si="19" xml:space="preserve"> J41/F41</f>
+        <v>1.0851088055695444</v>
+      </c>
+      <c r="L41" s="7">
+        <v>6</v>
+      </c>
+      <c r="M41" s="6">
+        <f t="shared" ref="M41:M44" si="20" xml:space="preserve"> J41/F41^2</f>
+        <v>0.90425733797462027</v>
+      </c>
       <c r="N41" s="7"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="4">
+        <f>B39*B41/298</f>
+        <v>0.25671140939597314</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="15"/>
+        <v>1.3033999999999999</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="16"/>
+        <v>-9.6600000000000019E-2</v>
+      </c>
+      <c r="I42" s="4">
+        <f t="shared" si="17"/>
+        <v>-1834.3764358153132</v>
+      </c>
+      <c r="J42" s="6">
+        <f t="shared" si="18"/>
+        <v>1.7470251769669649</v>
+      </c>
+      <c r="K42" s="6">
+        <f t="shared" si="19"/>
+        <v>1.247875126404975</v>
+      </c>
+      <c r="L42" s="7">
+        <v>6.9</v>
+      </c>
+      <c r="M42" s="6">
+        <f t="shared" si="20"/>
+        <v>0.89133937600355362</v>
+      </c>
       <c r="N42" s="7"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="4">
+        <f>$B$3/B42</f>
+        <v>2.7535135610875244E-5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="2">
+        <v>4</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="15"/>
+        <v>1.4752000000000001</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="16"/>
+        <v>-0.12480000000000002</v>
+      </c>
+      <c r="I43" s="4">
+        <f t="shared" si="17"/>
+        <v>-2369.8776313638828</v>
+      </c>
+      <c r="J43" s="6">
+        <f t="shared" si="18"/>
+        <v>2.2570263155846502</v>
+      </c>
+      <c r="K43" s="6">
+        <f t="shared" si="19"/>
+        <v>1.4106414472404063</v>
+      </c>
+      <c r="L43" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="M43" s="6">
+        <f t="shared" si="20"/>
+        <v>0.88165090452525385</v>
+      </c>
       <c r="N43" s="7"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E44" s="2">
+        <v>5</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="15"/>
+        <v>1.6434000000000002</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="16"/>
+        <v>-0.15659999999999985</v>
+      </c>
+      <c r="I44" s="4">
+        <f t="shared" si="17"/>
+        <v>-2973.7406816633302</v>
+      </c>
+      <c r="J44" s="6">
+        <f t="shared" si="18"/>
+        <v>2.8321339825365048</v>
+      </c>
+      <c r="K44" s="6">
+        <f t="shared" si="19"/>
+        <v>1.573407768075836</v>
+      </c>
+      <c r="L44" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="M44" s="6">
+        <f t="shared" si="20"/>
+        <v>0.87411542670879772</v>
+      </c>
       <c r="N44" s="7"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -9044,7 +9339,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N46" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -9067,11 +9362,11 @@
       </c>
       <c r="B50" s="6">
         <f xml:space="preserve"> $M$13</f>
-        <v>0.32553264167086327</v>
+        <v>1.211704832885989</v>
       </c>
       <c r="C50" s="6">
         <f>LN(B50)</f>
-        <v>-1.1222925407304634</v>
+        <v>0.19202832076433624</v>
       </c>
       <c r="D50">
         <f>-1/A50</f>
@@ -9086,11 +9381,11 @@
         <v>0.59</v>
       </c>
       <c r="C51" s="6">
-        <f t="shared" ref="C51:C52" si="18">LN(B51)</f>
+        <f t="shared" ref="C51:C52" si="21">LN(B51)</f>
         <v>-0.52763274208237199</v>
       </c>
       <c r="D51">
-        <f t="shared" ref="D51:D52" si="19">-1/A51</f>
+        <f t="shared" ref="D51:D52" si="22">-1/A51</f>
         <v>-2.0833333333333333E-3</v>
       </c>
     </row>
@@ -9102,11 +9397,11 @@
         <v>0.8</v>
       </c>
       <c r="C52" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>-0.22314355131420971</v>
       </c>
       <c r="D52">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>-1.9607843137254902E-3</v>
       </c>
     </row>

</xml_diff>